<commit_message>
final milestone one submission
</commit_message>
<xml_diff>
--- a/Blancos Milestone 1.xlsx
+++ b/Blancos Milestone 1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="289">
   <si>
     <t>Blancos</t>
   </si>
@@ -792,6 +792,9 @@
   </si>
   <si>
     <t>The error rate of users submitting their payment details at the checkout page mustn’t exceed 10%.</t>
+  </si>
+  <si>
+    <t>35, 36, 43</t>
   </si>
   <si>
     <t>Performance</t>
@@ -1214,7 +1217,7 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -1244,7 +1247,7 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -1277,7 +1280,7 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -5606,7 +5609,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" ht="28.5" customHeight="1">
+    <row r="40" ht="18.75" customHeight="1">
       <c r="A40" s="27" t="s">
         <v>109</v>
       </c>
@@ -5650,7 +5653,7 @@
       <c r="Y40" s="36"/>
       <c r="Z40" s="36"/>
     </row>
-    <row r="41" ht="27.0" customHeight="1">
+    <row r="41" ht="16.5" customHeight="1">
       <c r="A41" s="27" t="s">
         <v>109</v>
       </c>
@@ -5676,7 +5679,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" ht="27.0" customHeight="1">
+    <row r="42" ht="18.75" customHeight="1">
       <c r="A42" s="27" t="s">
         <v>109</v>
       </c>
@@ -5700,7 +5703,7 @@
       </c>
       <c r="H42" s="20"/>
     </row>
-    <row r="43" ht="27.0" customHeight="1">
+    <row r="43" ht="19.5" customHeight="1">
       <c r="A43" s="27" t="s">
         <v>109</v>
       </c>
@@ -5724,7 +5727,7 @@
       </c>
       <c r="H43" s="20"/>
     </row>
-    <row r="44" ht="27.0" customHeight="1">
+    <row r="44" ht="17.25" customHeight="1">
       <c r="A44" s="27" t="s">
         <v>109</v>
       </c>
@@ -5748,7 +5751,7 @@
       </c>
       <c r="H44" s="20"/>
     </row>
-    <row r="45" ht="26.25" customHeight="1">
+    <row r="45" ht="17.25" customHeight="1">
       <c r="A45" s="37" t="s">
         <v>109</v>
       </c>
@@ -5772,7 +5775,7 @@
       </c>
       <c r="H45" s="20"/>
     </row>
-    <row r="46" ht="28.5" customHeight="1">
+    <row r="46" ht="16.5" customHeight="1">
       <c r="A46" s="27" t="s">
         <v>109</v>
       </c>
@@ -10300,7 +10303,7 @@
     <col customWidth="1" min="1" max="1" width="19.25"/>
     <col customWidth="1" min="2" max="2" width="16.13"/>
     <col customWidth="1" min="3" max="3" width="93.25"/>
-    <col customWidth="1" min="4" max="4" width="118.63"/>
+    <col customWidth="1" min="4" max="4" width="132.13"/>
     <col customWidth="1" min="5" max="5" width="27.25"/>
     <col customWidth="1" min="6" max="6" width="51.88"/>
   </cols>
@@ -10361,8 +10364,8 @@
       <c r="E2" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="58">
-        <v>26.0</v>
+      <c r="F2" s="58" t="s">
+        <v>258</v>
       </c>
       <c r="G2" s="59"/>
       <c r="H2" s="60"/>
@@ -10390,19 +10393,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E3" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="58">
-        <v>27.0</v>
+        <v>44.0</v>
       </c>
       <c r="G3" s="59"/>
       <c r="H3" s="60"/>
@@ -10430,19 +10433,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D4" s="56" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E4" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="58">
-        <v>27.0</v>
+        <v>45.0</v>
       </c>
       <c r="G4" s="59"/>
       <c r="H4" s="60"/>
@@ -10470,19 +10473,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E5" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="58">
-        <v>28.0</v>
+        <v>45.0</v>
       </c>
       <c r="G5" s="59"/>
       <c r="H5" s="60"/>
@@ -10510,19 +10513,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E6" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="58">
-        <v>29.0</v>
+        <v>46.0</v>
       </c>
       <c r="G6" s="59"/>
       <c r="H6" s="60"/>
@@ -10550,19 +10553,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C7" s="56" t="s">
         <v>144</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E7" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="58">
-        <v>32.0</v>
+        <v>49.0</v>
       </c>
       <c r="G7" s="59"/>
       <c r="H7" s="60"/>
@@ -10590,19 +10593,19 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E8" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="58" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G8" s="59"/>
       <c r="H8" s="60"/>
@@ -10630,19 +10633,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C9" s="56" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D9" s="56" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E9" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="58">
-        <v>32.0</v>
+        <v>49.0</v>
       </c>
       <c r="G9" s="59"/>
       <c r="H9" s="60"/>
@@ -10670,19 +10673,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E10" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="58">
-        <v>31.0</v>
+        <v>48.0</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="60"/>
@@ -10710,19 +10713,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D11" s="56" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E11" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="58">
-        <v>30.0</v>
+        <v>47.0</v>
       </c>
       <c r="G11" s="59"/>
       <c r="H11" s="60"/>
@@ -10750,19 +10753,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D12" s="56" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E12" s="61" t="s">
         <v>39</v>
       </c>
       <c r="F12" s="58">
-        <v>30.0</v>
+        <v>47.0</v>
       </c>
       <c r="G12" s="59"/>
       <c r="H12" s="60"/>

</xml_diff>